<commit_message>
carga masiva de productos y precio
</commit_message>
<xml_diff>
--- a/public/archivos/formato_carga_masiva_productos.xlsx
+++ b/public/archivos/formato_carga_masiva_productos.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
-  <si>
-    <t>Tabla 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+  <si>
+    <t>formato_carga_masiva_productos.xlsx - H</t>
   </si>
   <si>
     <t>Clave</t>
@@ -22,10 +22,10 @@
     <t>Proveedor</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>Subcategoria</t>
+    <t>Tipo de Producto</t>
+  </si>
+  <si>
+    <t>Categoria de Productos</t>
   </si>
   <si>
     <t>Precio</t>
@@ -82,10 +82,31 @@
     <t>Backing</t>
   </si>
   <si>
-    <t>BRANTANO</t>
-  </si>
-  <si>
-    <t>TELA PARA DECORACION</t>
+    <t>4268-05</t>
+  </si>
+  <si>
+    <t>Brentano</t>
+  </si>
+  <si>
+    <t>Telas Contract</t>
+  </si>
+  <si>
+    <t>Cortineros</t>
+  </si>
+  <si>
+    <t>Pranayama</t>
+  </si>
+  <si>
+    <t>Brass Bell</t>
+  </si>
+  <si>
+    <t>59" [ 150 cm ]</t>
+  </si>
+  <si>
+    <t>100% Solution-Dyed Acrylic</t>
+  </si>
+  <si>
+    <t>alta</t>
   </si>
 </sst>
 </file>
@@ -113,7 +134,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,14 +153,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -207,96 +222,39 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -315,10 +273,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fffff056"/>
+      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
@@ -1348,16 +1305,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:V22"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="22" width="16.3516" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.67188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.67188" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.8516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1719" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6719" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.35156" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85156" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.3516" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85156" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.3516" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.1719" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1386,7 +1365,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" ht="32.25" customHeight="1">
+    <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
@@ -1396,83 +1375,95 @@
       <c r="C2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" t="s" s="3">
         <v>4</v>
       </c>
       <c r="E2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="4">
+      <c r="G2" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="4">
+      <c r="H2" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="4">
+      <c r="I2" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="J2" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="4">
+      <c r="K2" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="4">
+      <c r="L2" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="M2" t="s" s="4">
+      <c r="M2" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="N2" t="s" s="4">
+      <c r="N2" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="O2" t="s" s="4">
+      <c r="O2" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="P2" t="s" s="4">
+      <c r="P2" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="Q2" t="s" s="4">
+      <c r="Q2" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="R2" t="s" s="4">
+      <c r="R2" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="S2" t="s" s="4">
+      <c r="S2" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="T2" t="s" s="4">
+      <c r="T2" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="U2" t="s" s="4">
+      <c r="U2" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="V2" t="s" s="4">
+      <c r="V2" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="3" ht="32.25" customHeight="1">
-      <c r="A3" s="5">
-        <v>1234</v>
-      </c>
-      <c r="B3" t="s" s="6">
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="B3" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="C3" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="E3" s="7">
+        <v>220</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s" s="6">
+        <v>31</v>
+      </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1486,468 +1477,12 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="12"/>
-      <c r="T20" s="12"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="12"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
feat: added fields to cargamasiva productos
</commit_message>
<xml_diff>
--- a/public/archivos/formato_carga_masiva_productos.xlsx
+++ b/public/archivos/formato_carga_masiva_productos.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Desktop\789.mx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDD8E0F2-236D-4A1B-B02F-50CBB1EDD114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>formato_carga_masiva_productos.xlsx - H</t>
   </si>
@@ -107,15 +116,21 @@
   </si>
   <si>
     <t>alta</t>
+  </si>
+  <si>
+    <t>Precio Residencial</t>
+  </si>
+  <si>
+    <t>Precio Comercial</t>
+  </si>
+  <si>
+    <t>Precio Distribuidor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -128,7 +143,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -224,37 +239,37 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -264,26 +279,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -482,7 +556,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -500,7 +574,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -529,7 +603,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -554,7 +628,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -579,7 +653,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +678,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -629,7 +703,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -654,7 +728,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -679,7 +753,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -704,7 +778,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -729,7 +803,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -742,9 +816,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -761,7 +841,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -779,7 +859,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,7 +884,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -829,7 +909,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -854,7 +934,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -879,7 +959,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,7 +984,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +1009,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -954,7 +1034,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1059,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1004,7 +1084,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,9 +1097,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1033,7 +1119,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1051,7 +1137,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1080,7 +1166,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1105,7 +1191,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1216,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1241,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,7 +1266,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,7 +1291,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1230,7 +1316,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1255,7 +1341,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1280,7 +1366,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1293,196 +1379,230 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.67188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.67188" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.8516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6719" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1719" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6719" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.35156" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85156" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.3516" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85156" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.3516" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11.1719" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.44140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="9.88671875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11.21875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="8" style="1" customWidth="1"/>
+    <col min="26" max="26" width="8.33203125" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:25" ht="27.6" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="M2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="O2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="P2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="Q2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="S2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" t="s" s="3">
+      <c r="T2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R2" t="s" s="3">
+      <c r="U2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S2" t="s" s="3">
+      <c r="V2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T2" t="s" s="3">
+      <c r="W2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U2" t="s" s="3">
+      <c r="X2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V2" t="s" s="3">
+      <c r="Y2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>220</v>
       </c>
-      <c r="F3" t="s" s="6">
+      <c r="F3" s="6">
+        <v>250</v>
+      </c>
+      <c r="G3" s="6">
+        <v>245</v>
+      </c>
+      <c r="H3" s="6">
+        <v>240</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G3" t="s" s="6">
+      <c r="J3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s" s="6">
+      <c r="K3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="L3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J3" t="s" s="6">
+      <c r="M3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:Y1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>